<commit_message>
Added readme.md files for all the directories.
</commit_message>
<xml_diff>
--- a/FlockAuditLogs/SPDSearchAuditLogs.xlsx
+++ b/FlockAuditLogs/SPDSearchAuditLogs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uoecs-my.sharepoint.com/personal/sethm_uoecs_org/Documents/Personal/EOE/repos/springfield-oregon/FlockAuditLogs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="138" documentId="8_{DAB02105-A862-4746-A575-54ACFCCFC9A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4BD91A66-844F-4DE8-ACFE-215DAD585F9F}"/>
+  <xr:revisionPtr revIDLastSave="139" documentId="8_{DAB02105-A862-4746-A575-54ACFCCFC9A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6982F085-DEBC-4C8F-B8FF-E7953E111695}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-1755" windowWidth="29040" windowHeight="17520" xr2:uid="{B6240E8A-A065-4699-990A-FB137E45CDF7}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{B6240E8A-A065-4699-990A-FB137E45CDF7}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="4" r:id="rId1"/>
@@ -20,7 +20,7 @@
   </sheets>
   <calcPr calcId="0"/>
   <pivotCaches>
-    <pivotCache cacheId="7" r:id="rId5"/>
+    <pivotCache cacheId="0" r:id="rId5"/>
   </pivotCaches>
 </workbook>
 </file>
@@ -15278,7 +15278,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{E167D0F0-6A2D-4929-8EE4-C5F88AFA6B22}" name="PivotTable2" cacheId="7" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="UserId">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{E167D0F0-6A2D-4929-8EE4-C5F88AFA6B22}" name="PivotTable2" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="UserId">
   <location ref="A3:B42" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="7">
     <pivotField dataField="1" showAll="0"/>
@@ -19183,7 +19183,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{5B184307-B41F-4E99-B621-2E102899AA8B}" name="PivotTable3" cacheId="7" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{5B184307-B41F-4E99-B621-2E102899AA8B}" name="PivotTable3" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:B98" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="7">
     <pivotField dataField="1" showAll="0"/>
@@ -23123,7 +23123,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D36EA656-2B9B-4C78-9AD1-E518CED12845}">
   <dimension ref="A1:A8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
@@ -23172,9 +23172,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC5116CA-05B5-4468-B087-85841270E5BD}">
   <dimension ref="A1:E1297"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A172" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C193" sqref="C193"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -26458,7 +26458,7 @@
         <v>29</v>
       </c>
       <c r="C193" s="7">
-        <v>45859.931211446761</v>
+        <v>45859.931215277778</v>
       </c>
       <c r="D193">
         <v>3</v>

</xml_diff>